<commit_message>
atualizações na ata semanal
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/ATA-Semana-2A.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/ATA-Semana-2A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4fd29038e46714d/Área de Trabalho/SPTECH/Pesquisa e Inovação/Sprint-SPTECH/ATAs_de_Reuniao/Sprint 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="13_ncr:1_{57DF1821-0962-4C64-A1D3-54AC52FF73A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96456C09-10E5-45BB-B3E2-6B9469741225}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="13_ncr:1_{57DF1821-0962-4C64-A1D3-54AC52FF73A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{062789DF-1572-4A7B-A380-A86BA933DC0B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="1" activeTab="7" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="65">
   <si>
     <t>NOME</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>INCREMENTAR O TRELLO</t>
+  </si>
+  <si>
+    <t>DIAGRAMA DE NEGÓCIO</t>
   </si>
 </sst>
 </file>
@@ -754,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -799,6 +802,34 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -854,95 +885,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -952,16 +894,46 @@
     <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -973,15 +945,28 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1316,87 +1301,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1533,6 +1437,87 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -3150,18 +3135,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D11" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
   <autoFilter ref="A7:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I16" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
-  <autoFilter ref="F7:I16" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I17" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+  <autoFilter ref="F7:I17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I17">
+    <sortCondition ref="H7:H17"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="36"/>
     <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="35"/>
@@ -3651,21 +3639,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -3799,46 +3787,46 @@
     </row>
     <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
     </row>
     <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
     </row>
     <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="12" t="s">
         <v>20</v>
       </c>
@@ -4012,21 +4000,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -4160,46 +4148,46 @@
     </row>
     <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
     </row>
     <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
     </row>
     <row r="18" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
     </row>
     <row r="19" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="12" t="s">
         <v>20</v>
       </c>
@@ -4371,21 +4359,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -4501,46 +4489,46 @@
     </row>
     <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
     </row>
     <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="12" t="s">
         <v>20</v>
       </c>
@@ -4712,21 +4700,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -4842,46 +4830,46 @@
     </row>
     <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
     </row>
     <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="12" t="s">
         <v>20</v>
       </c>
@@ -5053,21 +5041,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -5183,46 +5171,46 @@
     </row>
     <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
     </row>
     <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="12" t="s">
         <v>20</v>
       </c>
@@ -5396,21 +5384,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -5526,46 +5514,46 @@
     </row>
     <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
     </row>
     <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="12" t="s">
         <v>20</v>
       </c>
@@ -5726,7 +5714,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5744,408 +5732,402 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="F3" s="14" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="F3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="36"/>
-      <c r="F4" s="31" t="s">
+      <c r="C4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="F4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="36"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="37"/>
-      <c r="F5" s="32" t="s">
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="F5" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="37"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="55"/>
     </row>
     <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="45" t="s">
+      <c r="I7" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="6">
         <v>45559</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="6">
+        <v>45567</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="33">
+      <c r="B9" s="6">
+        <v>45559</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="6">
         <v>45567</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="H9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45559</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="6">
+        <v>45567</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45555</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="6">
+        <v>45567</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I11" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="33">
-        <v>45559</v>
-      </c>
-      <c r="C9" s="47" t="s">
+    <row r="12" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="19"/>
+      <c r="D12" s="18"/>
+      <c r="F12" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="6">
+        <v>45567</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="33">
+      <c r="I12" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="F13" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="6">
         <v>45567</v>
       </c>
-      <c r="H9" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="48" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="33">
-        <v>45559</v>
-      </c>
-      <c r="C10" s="47" t="s">
+      <c r="H13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="F14" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="6">
+        <v>45567</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="33">
+      <c r="I14" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
+      <c r="F15" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="6">
         <v>45567</v>
       </c>
-      <c r="H10" s="47" t="s">
+      <c r="H15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I15" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="33">
-        <v>45555</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="33">
+    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
+      <c r="F16" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="6">
         <v>45567</v>
       </c>
-      <c r="H11" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="48" t="s">
+      <c r="H16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="40"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="35"/>
-      <c r="F12" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="33">
+    <row r="17" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
+      <c r="F17" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="6">
         <v>45567</v>
       </c>
-      <c r="H12" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="48" t="s">
+      <c r="H17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="F13" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="33">
-        <v>45567</v>
-      </c>
-      <c r="H13" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="F14" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="33">
-        <v>45567</v>
-      </c>
-      <c r="H14" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="25"/>
-      <c r="F15" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="33">
-        <v>45567</v>
-      </c>
-      <c r="H15" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="25"/>
-      <c r="F16" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="33">
-        <v>45567</v>
-      </c>
-      <c r="H16" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-    </row>
-    <row r="18" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="29"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="30"/>
-      <c r="F18"/>
-      <c r="G18"/>
-    </row>
-    <row r="19" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="66" t="s">
+    <row r="18" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="14"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="68"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="65" t="s">
+    <row r="20" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="70" t="s">
+      <c r="B20" s="47"/>
+      <c r="C20" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="71"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="62" t="s">
+      <c r="F20"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63" t="s">
+      <c r="B21" s="49"/>
+      <c r="C21" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="64"/>
-    </row>
-    <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="55" t="s">
+      <c r="D21" s="61"/>
+    </row>
+    <row r="22" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="50" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="51"/>
       <c r="C22" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="56"/>
-    </row>
-    <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="53" t="s">
+      <c r="D22" s="62"/>
+    </row>
+    <row r="23" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50" t="s">
+      <c r="B23" s="42"/>
+      <c r="C23" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="54"/>
-    </row>
-    <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="57" t="s">
+      <c r="D23" s="43"/>
+    </row>
+    <row r="24" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52" t="s">
+      <c r="B24" s="44"/>
+      <c r="C24" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="58"/>
-    </row>
-    <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="53" t="s">
+      <c r="D24" s="45"/>
+    </row>
+    <row r="25" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50" t="s">
+      <c r="B25" s="42"/>
+      <c r="C25" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="54"/>
-    </row>
-    <row r="26" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="59" t="s">
+      <c r="D25" s="43"/>
+    </row>
+    <row r="26" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60" t="s">
+      <c r="B26" s="40"/>
+      <c r="C26" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="61"/>
+      <c r="D26" s="41"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:D17"/>
@@ -6154,9 +6136,25 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="D8:D11 I8:I16">
+  <conditionalFormatting sqref="D8:D11 I8:I17">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
@@ -6180,7 +6178,7 @@
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D8:D11 I8:I16</xm:sqref>
+          <xm:sqref>D8:D11 I8:I17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8EFBC24D-2650-46F5-BA77-660A84572B57}">
           <x14:formula1>
@@ -6192,13 +6190,13 @@
           <x14:formula1>
             <xm:f>Quarta!$A$21:$A$26</xm:f>
           </x14:formula1>
-          <xm:sqref>B4:B5 G4:G5 G19</xm:sqref>
+          <xm:sqref>B4:B5 G4:G5 G20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CB2ECE66-384A-4231-9DE0-EE40A3A51602}">
           <x14:formula1>
             <xm:f>Quinta!$A$22:$A$27</xm:f>
           </x14:formula1>
-          <xm:sqref>H8:H16</xm:sqref>
+          <xm:sqref>H8:H17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>